<commit_message>
Data from the java implementation added, change on the code to match image files
</commit_message>
<xml_diff>
--- a/Datos Proyecto Final C#.xlsx
+++ b/Datos Proyecto Final C#.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\Documents\UNIVERSIDAD 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c\Desktop\universidad\Semestre8(tiempo)\Arqui-hard\ProyectoFinal-ArquiHard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07191302-B837-4E2E-8A01-28E41C83AEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A09AA1-D199-4B3C-9D0A-68462E845242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7037D96-2046-4484-9B87-9C9E2FB113E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D7037D96-2046-4484-9B87-9C9E2FB113E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -525,68 +524,68 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231FF977-868E-4ECE-9613-07B66D6A856E}">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,51 +924,51 @@
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
-      <c r="B2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40" t="s">
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="39" t="s">
         <v>5</v>
       </c>
     </row>
@@ -996,15 +995,15 @@
       <c r="H4" s="32">
         <v>234772700</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="41">
         <f>F4/($O$4*$O$4)</f>
         <v>1500.3775000000001</v>
       </c>
-      <c r="J4" s="49">
+      <c r="J4" s="42">
         <f>G4/($O$4*$O$4)</f>
         <v>1658.9337499999999</v>
       </c>
-      <c r="K4" s="50">
+      <c r="K4" s="43">
         <f>H4/($O$4*$O$4)</f>
         <v>1467.329375</v>
       </c>
@@ -1038,15 +1037,15 @@
       <c r="H5" s="30">
         <v>628145300</v>
       </c>
-      <c r="I5" s="51">
+      <c r="I5" s="44">
         <f t="shared" ref="I5:I8" si="0">F5/($O$4*$O$4)</f>
         <v>4380.4624999999996</v>
       </c>
-      <c r="J5" s="52">
+      <c r="J5" s="45">
         <f t="shared" ref="J5:J8" si="1">G5/($O$4*$O$4)</f>
         <v>4607.1868750000003</v>
       </c>
-      <c r="K5" s="53">
+      <c r="K5" s="46">
         <f t="shared" ref="K5:K8" si="2">H5/($O$4*$O$4)</f>
         <v>3925.9081249999999</v>
       </c>
@@ -1080,15 +1079,15 @@
       <c r="H6" s="30">
         <v>232111900</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="44">
         <f t="shared" si="0"/>
         <v>1551.105</v>
       </c>
-      <c r="J6" s="52">
+      <c r="J6" s="45">
         <f t="shared" si="1"/>
         <v>1595.5943749999999</v>
       </c>
-      <c r="K6" s="53">
+      <c r="K6" s="46">
         <f t="shared" si="2"/>
         <v>1450.6993749999999</v>
       </c>
@@ -1122,15 +1121,15 @@
       <c r="H7" s="30">
         <v>462551100</v>
       </c>
-      <c r="I7" s="51">
+      <c r="I7" s="44">
         <f t="shared" si="0"/>
         <v>3231.2449999999999</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="45">
         <f t="shared" si="1"/>
         <v>3097.1768750000001</v>
       </c>
-      <c r="K7" s="53">
+      <c r="K7" s="46">
         <f t="shared" si="2"/>
         <v>2890.944375</v>
       </c>
@@ -1164,15 +1163,15 @@
       <c r="H8" s="31">
         <v>225806500</v>
       </c>
-      <c r="I8" s="54">
+      <c r="I8" s="47">
         <f t="shared" si="0"/>
         <v>1534.5525</v>
       </c>
-      <c r="J8" s="55">
+      <c r="J8" s="48">
         <f t="shared" si="1"/>
         <v>1483.9525000000001</v>
       </c>
-      <c r="K8" s="56">
+      <c r="K8" s="49">
         <f t="shared" si="2"/>
         <v>1411.2906250000001</v>
       </c>
@@ -1206,15 +1205,15 @@
       <c r="H9" s="32">
         <v>653255300</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="41">
         <f>F9/($O$5*$O$5)</f>
         <v>1614.3883673469388</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="42">
         <f t="shared" ref="J9:K9" si="3">G9/($O$5*$O$5)</f>
         <v>1569.8512244897959</v>
       </c>
-      <c r="K9" s="50">
+      <c r="K9" s="43">
         <f t="shared" si="3"/>
         <v>1333.174081632653</v>
       </c>
@@ -1248,15 +1247,15 @@
       <c r="H10" s="30">
         <v>1948416500</v>
       </c>
-      <c r="I10" s="51">
+      <c r="I10" s="44">
         <f t="shared" ref="I10:I13" si="4">F10/($O$5*$O$5)</f>
         <v>4359.724487755102</v>
       </c>
-      <c r="J10" s="52">
+      <c r="J10" s="45">
         <f t="shared" ref="J10:J13" si="5">G10/($O$5*$O$5)</f>
         <v>3968.1912244897958</v>
       </c>
-      <c r="K10" s="53">
+      <c r="K10" s="46">
         <f t="shared" ref="K10:K13" si="6">H10/($O$5*$O$5)</f>
         <v>3976.3602040816327</v>
       </c>
@@ -1290,15 +1289,15 @@
       <c r="H11" s="30">
         <v>642292300</v>
       </c>
-      <c r="I11" s="51">
+      <c r="I11" s="44">
         <f t="shared" si="4"/>
         <v>1529.8455102040816</v>
       </c>
-      <c r="J11" s="52">
+      <c r="J11" s="45">
         <f t="shared" si="5"/>
         <v>1467.8520408163265</v>
       </c>
-      <c r="K11" s="53">
+      <c r="K11" s="46">
         <f t="shared" si="6"/>
         <v>1310.800612244898</v>
       </c>
@@ -1332,15 +1331,15 @@
       <c r="H12" s="30">
         <v>1303122300</v>
       </c>
-      <c r="I12" s="51">
+      <c r="I12" s="44">
         <f t="shared" si="4"/>
         <v>3047.5963265306123</v>
       </c>
-      <c r="J12" s="52">
+      <c r="J12" s="45">
         <f t="shared" si="5"/>
         <v>2634.03</v>
       </c>
-      <c r="K12" s="53">
+      <c r="K12" s="46">
         <f t="shared" si="6"/>
         <v>2659.4332653061224</v>
       </c>
@@ -1368,15 +1367,15 @@
       <c r="H13" s="31">
         <v>625238000</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="47">
         <f t="shared" si="4"/>
         <v>1510.9583673469388</v>
       </c>
-      <c r="J13" s="55">
+      <c r="J13" s="48">
         <f t="shared" si="5"/>
         <v>1394.5253061224489</v>
       </c>
-      <c r="K13" s="56">
+      <c r="K13" s="49">
         <f t="shared" si="6"/>
         <v>1275.995918367347</v>
       </c>
@@ -1404,15 +1403,15 @@
       <c r="H14" s="32">
         <v>1317597800</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="41">
         <f>F14/($O$6*$O$6)</f>
         <v>1500.2715000000001</v>
       </c>
-      <c r="J14" s="49">
+      <c r="J14" s="42">
         <f t="shared" ref="J14:K14" si="7">G14/($O$6*$O$6)</f>
         <v>1332.7726</v>
       </c>
-      <c r="K14" s="50">
+      <c r="K14" s="43">
         <f t="shared" si="7"/>
         <v>1317.5978</v>
       </c>
@@ -1440,15 +1439,15 @@
       <c r="H15" s="30">
         <v>3993332700</v>
       </c>
-      <c r="I15" s="51">
+      <c r="I15" s="44">
         <f t="shared" ref="I15:I18" si="8">F15/($O$6*$O$6)</f>
         <v>4179.3334990000003</v>
       </c>
-      <c r="J15" s="52">
+      <c r="J15" s="45">
         <f t="shared" ref="J15:J18" si="9">G15/($O$6*$O$6)</f>
         <v>3893.3962999999999</v>
       </c>
-      <c r="K15" s="53">
+      <c r="K15" s="46">
         <f t="shared" ref="K15:K18" si="10">H15/($O$6*$O$6)</f>
         <v>3993.3326999999999</v>
       </c>
@@ -1476,15 +1475,15 @@
       <c r="H16" s="30">
         <v>1278404500</v>
       </c>
-      <c r="I16" s="51">
+      <c r="I16" s="44">
         <f t="shared" si="8"/>
         <v>1469.0785000000001</v>
       </c>
-      <c r="J16" s="52">
+      <c r="J16" s="45">
         <f t="shared" si="9"/>
         <v>1283.1648</v>
       </c>
-      <c r="K16" s="53">
+      <c r="K16" s="46">
         <f t="shared" si="10"/>
         <v>1278.4045000000001</v>
       </c>
@@ -1512,15 +1511,15 @@
       <c r="H17" s="30">
         <v>2631046000</v>
       </c>
-      <c r="I17" s="51">
+      <c r="I17" s="44">
         <f t="shared" si="8"/>
         <v>2836.8933000000002</v>
       </c>
-      <c r="J17" s="52">
+      <c r="J17" s="45">
         <f t="shared" si="9"/>
         <v>2619.5911000000001</v>
       </c>
-      <c r="K17" s="53">
+      <c r="K17" s="46">
         <f t="shared" si="10"/>
         <v>2631.0459999999998</v>
       </c>
@@ -1548,15 +1547,15 @@
       <c r="H18" s="31">
         <v>1234940600</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I18" s="47">
         <f t="shared" si="8"/>
         <v>1417.4949999999999</v>
       </c>
-      <c r="J18" s="55">
+      <c r="J18" s="48">
         <f t="shared" si="9"/>
         <v>1263.1358</v>
       </c>
-      <c r="K18" s="56">
+      <c r="K18" s="49">
         <f t="shared" si="10"/>
         <v>1234.9405999999999</v>
       </c>
@@ -1584,15 +1583,15 @@
       <c r="H19" s="32">
         <v>2222830000</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="41">
         <f>F19/($O$7*$O$7)</f>
         <v>1439.6017159763314</v>
       </c>
-      <c r="J19" s="49">
+      <c r="J19" s="42">
         <f t="shared" ref="J19:K19" si="11">G19/($O$7*$O$7)</f>
         <v>1305.5250295857988</v>
       </c>
-      <c r="K19" s="50">
+      <c r="K19" s="43">
         <f t="shared" si="11"/>
         <v>1315.2840236686391</v>
       </c>
@@ -1620,16 +1619,16 @@
       <c r="H20" s="30">
         <v>6618000000</v>
       </c>
-      <c r="I20" s="51">
+      <c r="I20" s="44">
         <f t="shared" ref="I20:I23" si="12">F20/($O$7*$O$7)</f>
         <v>4089.4521301775148</v>
       </c>
-      <c r="J20" s="52">
-        <f>G20/($O$7*$O$7)</f>
+      <c r="J20" s="45">
+        <f t="shared" ref="J20:K23" si="13">G20/($O$7*$O$7)</f>
         <v>3921.1353254437868</v>
       </c>
-      <c r="K20" s="53">
-        <f>H20/($O$7*$O$7)</f>
+      <c r="K20" s="46">
+        <f t="shared" si="13"/>
         <v>3915.9763313609469</v>
       </c>
     </row>
@@ -1656,16 +1655,16 @@
       <c r="H21" s="30">
         <v>2177641800</v>
       </c>
-      <c r="I21" s="51">
+      <c r="I21" s="44">
         <f t="shared" si="12"/>
         <v>1412.5290532544379</v>
       </c>
-      <c r="J21" s="52">
-        <f>G21/($O$7*$O$7)</f>
+      <c r="J21" s="45">
+        <f t="shared" si="13"/>
         <v>1315.907100591716</v>
       </c>
-      <c r="K21" s="53">
-        <f>H21/($O$7*$O$7)</f>
+      <c r="K21" s="46">
+        <f t="shared" si="13"/>
         <v>1288.5454437869823</v>
       </c>
     </row>
@@ -1692,16 +1691,16 @@
       <c r="H22" s="30">
         <v>4419675700</v>
       </c>
-      <c r="I22" s="51">
+      <c r="I22" s="44">
         <f t="shared" si="12"/>
         <v>2752.4641420118342</v>
       </c>
-      <c r="J22" s="52">
-        <f>G22/($O$7*$O$7)</f>
+      <c r="J22" s="45">
+        <f t="shared" si="13"/>
         <v>2676.3718343195264</v>
       </c>
-      <c r="K22" s="53">
-        <f>H22/($O$7*$O$7)</f>
+      <c r="K22" s="46">
+        <f t="shared" si="13"/>
         <v>2615.1927218934911</v>
       </c>
     </row>
@@ -1728,16 +1727,16 @@
       <c r="H23" s="31">
         <v>2074279700</v>
       </c>
-      <c r="I23" s="54">
+      <c r="I23" s="47">
         <f t="shared" si="12"/>
         <v>1336.4487573964498</v>
       </c>
-      <c r="J23" s="55">
-        <f>G23/($O$7*$O$7)</f>
+      <c r="J23" s="48">
+        <f t="shared" si="13"/>
         <v>1243.6272781065088</v>
       </c>
-      <c r="K23" s="56">
-        <f>H23/($O$7*$O$7)</f>
+      <c r="K23" s="49">
+        <f t="shared" si="13"/>
         <v>1227.3844378698225</v>
       </c>
     </row>
@@ -1764,16 +1763,16 @@
       <c r="H24" s="32">
         <v>4764150700</v>
       </c>
-      <c r="I24" s="48">
+      <c r="I24" s="41">
         <f>F24/($O$8*$O$8)</f>
         <v>1951.7981640625001</v>
       </c>
-      <c r="J24" s="49">
-        <f t="shared" ref="J24:K24" si="13">G24/($O$8*$O$8)</f>
+      <c r="J24" s="42">
+        <f t="shared" ref="J24:K24" si="14">G24/($O$8*$O$8)</f>
         <v>1862.5713671875001</v>
       </c>
-      <c r="K24" s="50">
-        <f t="shared" si="13"/>
+      <c r="K24" s="43">
+        <f t="shared" si="14"/>
         <v>1860.9963671875</v>
       </c>
     </row>
@@ -1800,16 +1799,16 @@
       <c r="H25" s="30">
         <v>14354507900</v>
       </c>
-      <c r="I25" s="51">
-        <f t="shared" ref="I25:I28" si="14">F25/($O$8*$O$8)</f>
+      <c r="I25" s="44">
+        <f t="shared" ref="I25:I28" si="15">F25/($O$8*$O$8)</f>
         <v>5596.0928515625001</v>
       </c>
-      <c r="J25" s="52">
-        <f>G25/($O$8*$O$8)</f>
+      <c r="J25" s="45">
+        <f t="shared" ref="J25:K28" si="16">G25/($O$8*$O$8)</f>
         <v>5484.11328125</v>
       </c>
-      <c r="K25" s="53">
-        <f>H25/($O$8*$O$8)</f>
+      <c r="K25" s="46">
+        <f t="shared" si="16"/>
         <v>5607.2296484375001</v>
       </c>
     </row>
@@ -1836,16 +1835,16 @@
       <c r="H26" s="30">
         <v>4670425400</v>
       </c>
-      <c r="I26" s="51">
-        <f t="shared" si="14"/>
+      <c r="I26" s="44">
+        <f t="shared" si="15"/>
         <v>1928.4123046875</v>
       </c>
-      <c r="J26" s="52">
-        <f>G26/($O$8*$O$8)</f>
+      <c r="J26" s="45">
+        <f t="shared" si="16"/>
         <v>1856.952421875</v>
       </c>
-      <c r="K26" s="53">
-        <f>H26/($O$8*$O$8)</f>
+      <c r="K26" s="46">
+        <f t="shared" si="16"/>
         <v>1824.3849218749999</v>
       </c>
     </row>
@@ -1872,16 +1871,16 @@
       <c r="H27" s="30">
         <v>9506994900</v>
       </c>
-      <c r="I27" s="51">
-        <f t="shared" si="14"/>
+      <c r="I27" s="44">
+        <f t="shared" si="15"/>
         <v>3809.5188671874998</v>
       </c>
-      <c r="J27" s="52">
-        <f>G27/($O$8*$O$8)</f>
+      <c r="J27" s="45">
+        <f t="shared" si="16"/>
         <v>3706.7996484374999</v>
       </c>
-      <c r="K27" s="53">
-        <f>H27/($O$8*$O$8)</f>
+      <c r="K27" s="46">
+        <f t="shared" si="16"/>
         <v>3713.6698828125</v>
       </c>
     </row>
@@ -1908,16 +1907,16 @@
       <c r="H28" s="31">
         <v>4514280100</v>
       </c>
-      <c r="I28" s="54">
-        <f t="shared" si="14"/>
+      <c r="I28" s="47">
+        <f t="shared" si="15"/>
         <v>1841.5656640625</v>
       </c>
-      <c r="J28" s="55">
-        <f>G28/($O$8*$O$8)</f>
+      <c r="J28" s="48">
+        <f t="shared" si="16"/>
         <v>1787.3612499999999</v>
       </c>
-      <c r="K28" s="56">
-        <f>H28/($O$8*$O$8)</f>
+      <c r="K28" s="49">
+        <f t="shared" si="16"/>
         <v>1763.3906640625</v>
       </c>
     </row>
@@ -1944,16 +1943,16 @@
       <c r="H29" s="32">
         <v>7091473500</v>
       </c>
-      <c r="I29" s="48">
+      <c r="I29" s="41">
         <f>F29/($O$9*$O$9)</f>
         <v>2038.2696675900277</v>
       </c>
-      <c r="J29" s="49">
-        <f t="shared" ref="J29:K29" si="15">G29/($O$9*$O$9)</f>
+      <c r="J29" s="42">
+        <f t="shared" ref="J29:K29" si="17">G29/($O$9*$O$9)</f>
         <v>1875.4868698060941</v>
       </c>
-      <c r="K29" s="50">
-        <f t="shared" si="15"/>
+      <c r="K29" s="43">
+        <f t="shared" si="17"/>
         <v>1964.3970914127424</v>
       </c>
     </row>
@@ -1980,16 +1979,16 @@
       <c r="H30" s="30">
         <v>22181284000</v>
       </c>
-      <c r="I30" s="51">
+      <c r="I30" s="44">
         <f>F30/($O$9*$O$9)</f>
         <v>6054.7556509695287</v>
       </c>
-      <c r="J30" s="52">
-        <f>G30/($O$9*$O$9)</f>
+      <c r="J30" s="45">
+        <f t="shared" ref="J30:K33" si="18">G30/($O$9*$O$9)</f>
         <v>6036.6434626038781</v>
       </c>
-      <c r="K30" s="53">
-        <f>H30/($O$9*$O$9)</f>
+      <c r="K30" s="46">
+        <f t="shared" si="18"/>
         <v>6144.4</v>
       </c>
     </row>
@@ -2016,16 +2015,16 @@
       <c r="H31" s="30">
         <v>7503063300</v>
       </c>
-      <c r="I31" s="51">
+      <c r="I31" s="44">
         <f>F31/($O$9*$O$9)</f>
         <v>2164.6611634349028</v>
       </c>
-      <c r="J31" s="52">
-        <f>G31/($O$9*$O$9)</f>
+      <c r="J31" s="45">
+        <f t="shared" si="18"/>
         <v>1982.5936842105264</v>
       </c>
-      <c r="K31" s="53">
-        <f>H31/($O$9*$O$9)</f>
+      <c r="K31" s="46">
+        <f t="shared" si="18"/>
         <v>2078.4108864265927</v>
       </c>
     </row>
@@ -2052,16 +2051,16 @@
       <c r="H32" s="30">
         <v>13880629000</v>
       </c>
-      <c r="I32" s="51">
+      <c r="I32" s="44">
         <f>F32/($O$9*$O$9)</f>
         <v>3846.5707202216067</v>
       </c>
-      <c r="J32" s="52">
-        <f>G32/($O$9*$O$9)</f>
+      <c r="J32" s="45">
+        <f t="shared" si="18"/>
         <v>3840.6918282548477</v>
       </c>
-      <c r="K32" s="53">
-        <f>H32/($O$9*$O$9)</f>
+      <c r="K32" s="46">
+        <f t="shared" si="18"/>
         <v>3845.0495844875345</v>
       </c>
     </row>
@@ -2088,16 +2087,16 @@
       <c r="H33" s="31">
         <v>6678856500</v>
       </c>
-      <c r="I33" s="54">
+      <c r="I33" s="47">
         <f>F33/($O$9*$O$9)</f>
         <v>1924.4445429362881</v>
       </c>
-      <c r="J33" s="55">
-        <f>G33/($O$9*$O$9)</f>
+      <c r="J33" s="48">
+        <f t="shared" si="18"/>
         <v>1704.1749861495846</v>
       </c>
-      <c r="K33" s="56">
-        <f>H33/($O$9*$O$9)</f>
+      <c r="K33" s="49">
+        <f t="shared" si="18"/>
         <v>1850.0987534626038</v>
       </c>
     </row>
@@ -2124,16 +2123,16 @@
       <c r="H34" s="32">
         <v>10112609600</v>
       </c>
-      <c r="I34" s="48">
+      <c r="I34" s="41">
         <f>F34/($O$10*$O$10)</f>
         <v>2064.0631818181819</v>
       </c>
-      <c r="J34" s="49">
-        <f t="shared" ref="J34:K34" si="16">G34/($O$10*$O$10)</f>
+      <c r="J34" s="42">
+        <f t="shared" ref="J34:K34" si="19">G34/($O$10*$O$10)</f>
         <v>1986.1385950413223</v>
       </c>
-      <c r="K34" s="50">
-        <f t="shared" si="16"/>
+      <c r="K34" s="43">
+        <f t="shared" si="19"/>
         <v>2089.3821487603304</v>
       </c>
     </row>
@@ -2160,16 +2159,16 @@
       <c r="H35" s="30">
         <v>28674518600</v>
       </c>
-      <c r="I35" s="51">
-        <f t="shared" ref="I35:I38" si="17">F35/($O$10*$O$10)</f>
+      <c r="I35" s="44">
+        <f t="shared" ref="I35:I38" si="20">F35/($O$10*$O$10)</f>
         <v>5915.8175000000001</v>
       </c>
-      <c r="J35" s="52">
-        <f>G35/($O$10*$O$10)</f>
+      <c r="J35" s="45">
+        <f t="shared" ref="J35:K38" si="21">G35/($O$10*$O$10)</f>
         <v>5787.3849793388426</v>
       </c>
-      <c r="K35" s="53">
-        <f>H35/($O$10*$O$10)</f>
+      <c r="K35" s="46">
+        <f t="shared" si="21"/>
         <v>5924.4873140495865</v>
       </c>
     </row>
@@ -2196,16 +2195,16 @@
       <c r="H36" s="30">
         <v>9723846600</v>
       </c>
-      <c r="I36" s="51">
-        <f t="shared" si="17"/>
+      <c r="I36" s="44">
+        <f t="shared" si="20"/>
         <v>1943.3144214876033</v>
       </c>
-      <c r="J36" s="52">
-        <f>G36/($O$10*$O$10)</f>
+      <c r="J36" s="45">
+        <f t="shared" si="21"/>
         <v>2072.2527066115704</v>
       </c>
-      <c r="K36" s="53">
-        <f>H36/($O$10*$O$10)</f>
+      <c r="K36" s="46">
+        <f t="shared" si="21"/>
         <v>2009.0592148760331</v>
       </c>
     </row>
@@ -2232,16 +2231,16 @@
       <c r="H37" s="30">
         <v>19540771400</v>
       </c>
-      <c r="I37" s="51">
-        <f t="shared" si="17"/>
+      <c r="I37" s="44">
+        <f t="shared" si="20"/>
         <v>3922.4972520661158</v>
       </c>
-      <c r="J37" s="52">
-        <f>G37/($O$10*$O$10)</f>
+      <c r="J37" s="45">
+        <f t="shared" si="21"/>
         <v>3976.2037396694213</v>
       </c>
-      <c r="K37" s="53">
-        <f>H37/($O$10*$O$10)</f>
+      <c r="K37" s="46">
+        <f t="shared" si="21"/>
         <v>4037.3494628099174</v>
       </c>
     </row>
@@ -2268,16 +2267,16 @@
       <c r="H38" s="31">
         <v>9929941900</v>
       </c>
-      <c r="I38" s="54">
-        <f t="shared" si="17"/>
+      <c r="I38" s="47">
+        <f t="shared" si="20"/>
         <v>2116.6861570247934</v>
       </c>
-      <c r="J38" s="55">
-        <f>G38/($O$10*$O$10)</f>
+      <c r="J38" s="48">
+        <f t="shared" si="21"/>
         <v>2099.1812396694213</v>
       </c>
-      <c r="K38" s="56">
-        <f>H38/($O$10*$O$10)</f>
+      <c r="K38" s="49">
+        <f t="shared" si="21"/>
         <v>2051.6408884297521</v>
       </c>
     </row>
@@ -2304,16 +2303,16 @@
       <c r="H39" s="32">
         <v>12201900400</v>
       </c>
-      <c r="I39" s="48">
+      <c r="I39" s="41">
         <f>F39/($O$11*$O$11)</f>
         <v>1907.6102080000001</v>
       </c>
-      <c r="J39" s="49">
-        <f t="shared" ref="J39:K39" si="18">G39/($O$11*$O$11)</f>
+      <c r="J39" s="42">
+        <f t="shared" ref="J39:K39" si="22">G39/($O$11*$O$11)</f>
         <v>1961.8989280000001</v>
       </c>
-      <c r="K39" s="57">
-        <f t="shared" si="18"/>
+      <c r="K39" s="50">
+        <f t="shared" si="22"/>
         <v>1952.3040639999999</v>
       </c>
     </row>
@@ -2340,16 +2339,16 @@
       <c r="H40" s="30">
         <v>37111860500</v>
       </c>
-      <c r="I40" s="51">
-        <f t="shared" ref="I40:I43" si="19">F40/($O$11*$O$11)</f>
+      <c r="I40" s="44">
+        <f t="shared" ref="I40:I43" si="23">F40/($O$11*$O$11)</f>
         <v>5821.1597439999996</v>
       </c>
-      <c r="J40" s="52">
-        <f t="shared" ref="J40:J43" si="20">G40/($O$11*$O$11)</f>
+      <c r="J40" s="45">
+        <f t="shared" ref="J40:J43" si="24">G40/($O$11*$O$11)</f>
         <v>5790.9980320000004</v>
       </c>
-      <c r="K40" s="53">
-        <f t="shared" ref="K40:K43" si="21">H40/($O$11*$O$11)</f>
+      <c r="K40" s="46">
+        <f t="shared" ref="K40:K43" si="25">H40/($O$11*$O$11)</f>
         <v>5937.89768</v>
       </c>
     </row>
@@ -2376,16 +2375,16 @@
       <c r="H41" s="30">
         <v>11963727100</v>
       </c>
-      <c r="I41" s="51">
-        <f t="shared" si="19"/>
+      <c r="I41" s="44">
+        <f t="shared" si="23"/>
         <v>1911.757104</v>
       </c>
-      <c r="J41" s="52">
-        <f t="shared" si="20"/>
+      <c r="J41" s="45">
+        <f t="shared" si="24"/>
         <v>1960.045568</v>
       </c>
-      <c r="K41" s="53">
-        <f t="shared" si="21"/>
+      <c r="K41" s="46">
+        <f t="shared" si="25"/>
         <v>1914.196336</v>
       </c>
     </row>
@@ -2412,16 +2411,16 @@
       <c r="H42" s="30">
         <v>25309481700</v>
       </c>
-      <c r="I42" s="51">
-        <f t="shared" si="19"/>
+      <c r="I42" s="44">
+        <f t="shared" si="23"/>
         <v>3942.7717280000002</v>
       </c>
-      <c r="J42" s="52">
-        <f t="shared" si="20"/>
+      <c r="J42" s="45">
+        <f t="shared" si="24"/>
         <v>4013.725328</v>
       </c>
-      <c r="K42" s="53">
-        <f t="shared" si="21"/>
+      <c r="K42" s="46">
+        <f t="shared" si="25"/>
         <v>4049.5170720000001</v>
       </c>
     </row>
@@ -2439,7 +2438,7 @@
       <c r="E43" s="31">
         <v>5</v>
       </c>
-      <c r="F43" s="47">
+      <c r="F43" s="40">
         <v>12323467400</v>
       </c>
       <c r="G43" s="28">
@@ -2448,16 +2447,16 @@
       <c r="H43" s="31">
         <v>12373627100</v>
       </c>
-      <c r="I43" s="54">
-        <f t="shared" si="19"/>
+      <c r="I43" s="47">
+        <f t="shared" si="23"/>
         <v>1971.754784</v>
       </c>
-      <c r="J43" s="55">
-        <f t="shared" si="20"/>
+      <c r="J43" s="48">
+        <f t="shared" si="24"/>
         <v>1959.82376</v>
       </c>
-      <c r="K43" s="56">
-        <f t="shared" si="21"/>
+      <c r="K43" s="49">
+        <f t="shared" si="25"/>
         <v>1979.780336</v>
       </c>
     </row>

</xml_diff>